<commit_message>
anzahl schüler und schuhausgröse
</commit_message>
<xml_diff>
--- a/doc/data.xlsx
+++ b/doc/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA87A1F-0A96-4CE8-AE79-78566F66DC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49BD66A-64E9-4FFF-98F4-7A5D1363B136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{90DD26CF-6537-4991-AA6B-C99E48712A6F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{90DD26CF-6537-4991-AA6B-C99E48712A6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Hauptenergieträger der Heizung(en):</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>Ranking Strommix (1-gut, 2-mittel, 3-schlecht):</t>
+  </si>
+  <si>
+    <t>anzahl Schüler</t>
+  </si>
+  <si>
+    <t>Gebäudegrösse in Quadratmeter</t>
   </si>
 </sst>
 </file>
@@ -534,23 +540,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5B4877-3DAA-4E36-B79C-8123709474F3}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="73.1015625" customWidth="1"/>
-    <col min="2" max="2" width="28.41796875" customWidth="1"/>
+    <col min="1" max="1" width="73.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="18.7890625" customWidth="1"/>
-    <col min="5" max="5" width="15.62890625" customWidth="1"/>
-    <col min="6" max="6" width="20.47265625" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -567,7 +573,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -587,7 +593,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -607,11 +613,11 @@
         <v>32000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -631,7 +637,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -651,13 +657,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>33</v>
       </c>
@@ -677,7 +683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -697,7 +703,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="8" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" s="8" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
@@ -717,7 +723,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -737,11 +743,11 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -752,7 +758,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -763,7 +769,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -774,7 +780,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -785,11 +791,11 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -804,9 +810,49 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20">
+        <v>80</v>
+      </c>
+      <c r="C20">
+        <v>120</v>
+      </c>
+      <c r="D20">
+        <v>200</v>
+      </c>
+      <c r="E20">
+        <v>180</v>
+      </c>
+      <c r="F20">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21">
+        <v>170</v>
+      </c>
+      <c r="C21">
+        <v>200</v>
+      </c>
+      <c r="D21">
+        <v>250</v>
+      </c>
+      <c r="E21">
+        <v>240</v>
+      </c>
+      <c r="F21">
+        <v>300</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>